<commit_message>
sqm added for calculation which are done
</commit_message>
<xml_diff>
--- a/byhand/dvg_reo.xlsx
+++ b/byhand/dvg_reo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\workspace\kfintech\RealEstateAI\byhand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37134A68-6207-4E81-B2D8-185652BD1D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35816A64-FBAC-44E6-B2FA-D721BC726624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3558,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A63A6F5-31AB-4798-A958-181B73F691FF}">
   <dimension ref="A1:O153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4128,6 +4128,9 @@
       <c r="M12" s="2" t="s">
         <v>530</v>
       </c>
+      <c r="N12">
+        <v>310</v>
+      </c>
       <c r="O12" s="2" t="s">
         <v>527</v>
       </c>
@@ -4496,6 +4499,9 @@
       <c r="M20" s="2" t="s">
         <v>682</v>
       </c>
+      <c r="N20">
+        <v>419</v>
+      </c>
       <c r="O20" s="2" t="s">
         <v>680</v>
       </c>
@@ -7078,6 +7084,9 @@
       <c r="M75" s="2" t="s">
         <v>1031</v>
       </c>
+      <c r="N75">
+        <v>80</v>
+      </c>
       <c r="O75" s="2" t="s">
         <v>1028</v>
       </c>
@@ -7122,6 +7131,9 @@
       <c r="M76" s="2" t="s">
         <v>1035</v>
       </c>
+      <c r="N76">
+        <v>88</v>
+      </c>
       <c r="O76" s="2" t="s">
         <v>1033</v>
       </c>
@@ -8152,6 +8164,9 @@
       </c>
       <c r="M98" s="2" t="s">
         <v>877</v>
+      </c>
+      <c r="N98">
+        <v>200</v>
       </c>
       <c r="O98" s="2" t="s">
         <v>874</v>

</xml_diff>